<commit_message>
Update the features importance
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -813,61 +813,61 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2893169989624599</v>
+        <v>0.2893169989624623</v>
       </c>
       <c r="C2" t="n">
         <v>0.3943872552251285</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>RH_avg</t>
+          <t>Tn</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2506164845172168</v>
+        <v>0.1813592958955645</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1061353905077548</v>
+        <v>0.1816243256743412</v>
       </c>
       <c r="D3" t="n">
-        <v>1.05010614104517</v>
+        <v>0.4237924090919176</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Tn</t>
+          <t>RH_avg</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1813592958955493</v>
+        <v>0.2506164845172436</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1816243256743412</v>
+        <v>0.1061353905077548</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9516690740879611</v>
+        <v>0.2193522015595606</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>Tavg</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1304048800547974</v>
+        <v>0.06065280242151002</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02514024614723597</v>
+        <v>0.1052214880401069</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3050415355286802</v>
+        <v>0.2168771579026596</v>
       </c>
     </row>
     <row r="6">
@@ -877,61 +877,61 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0934029405706242</v>
+        <v>0.09340294057062298</v>
       </c>
       <c r="C6" t="n">
         <v>0.07972246640130111</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2910440705912866</v>
+        <v>0.1478203449511246</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Tavg</t>
+          <t>ff_avg</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.060652802421516</v>
+        <v>0.07646911220056765</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1052214880401069</v>
+        <v>0.06001532725417928</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2168771579026596</v>
+        <v>0.09444919051351454</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>ff_avg</t>
+          <t>ff_x</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07646911220057007</v>
+        <v>0.07142938879604899</v>
       </c>
       <c r="C8" t="n">
-        <v>0.06001532725417928</v>
+        <v>0.0477535007499524</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1636174731669034</v>
+        <v>0.06124153763408323</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>ff_x</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0714293887960535</v>
+        <v>0.1304048800547975</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0477535007499524</v>
+        <v>0.02514024614723597</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1083699754811857</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>